<commit_message>
Changes made to industry and linked for netzero-working-pre final fixes
</commit_message>
<xml_diff>
--- a/SATIM/DataSpreadsheets/TCH_GRNEXP.xlsx
+++ b/SATIM/DataSpreadsheets/TCH_GRNEXP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE\SATIM\DataSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BFD37EAD-83EB-49C8-B296-2E3D4F7485A7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{8692516F-34E6-4B11-BF20-B9864F34A823}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="796" firstSheet="1" activeTab="12" xr2:uid="{E4E4DEB2-CFB1-442C-9FC5-D51D154627BD}"/>
+    <workbookView xWindow="12915" yWindow="-17670" windowWidth="19200" windowHeight="14505" tabRatio="796" firstSheet="1" activeTab="12" xr2:uid="{E4E4DEB2-CFB1-442C-9FC5-D51D154627BD}"/>
   </bookViews>
   <sheets>
     <sheet name="ANSv2-692-Home" sheetId="9" r:id="rId1"/>
@@ -1971,7 +1971,7 @@
 </file>
 
 <file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D50-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2103,7 +2103,7 @@
 </file>
 
 <file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D50-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX20.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2191,7 +2191,7 @@
 </file>
 
 <file path=xl/activeX/activeX4.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D50-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX40.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2235,7 +2235,7 @@
 </file>
 
 <file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D50-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX50.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2467,9 +2467,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>247650</xdr:colOff>
+          <xdr:colOff>238125</xdr:colOff>
           <xdr:row>12</xdr:row>
-          <xdr:rowOff>114300</xdr:rowOff>
+          <xdr:rowOff>104775</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2525,9 +2525,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>238125</xdr:colOff>
+          <xdr:colOff>228600</xdr:colOff>
           <xdr:row>28</xdr:row>
-          <xdr:rowOff>85725</xdr:rowOff>
+          <xdr:rowOff>76200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2583,9 +2583,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>247650</xdr:colOff>
+          <xdr:colOff>238125</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>85725</xdr:rowOff>
+          <xdr:rowOff>76200</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2641,9 +2641,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>581025</xdr:colOff>
+          <xdr:colOff>571500</xdr:colOff>
           <xdr:row>17</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2699,9 +2699,9 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>561975</xdr:colOff>
+          <xdr:colOff>552450</xdr:colOff>
           <xdr:row>21</xdr:row>
-          <xdr:rowOff>152400</xdr:rowOff>
+          <xdr:rowOff>142875</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -2762,7 +2762,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>1314450</xdr:colOff>
+          <xdr:colOff>1304925</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>209550</xdr:rowOff>
         </xdr:to>
@@ -3584,7 +3584,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>2</xdr:col>
-          <xdr:colOff>647700</xdr:colOff>
+          <xdr:colOff>638175</xdr:colOff>
           <xdr:row>2</xdr:row>
           <xdr:rowOff>190500</xdr:rowOff>
         </xdr:to>
@@ -4682,7 +4682,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>6</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>95250</xdr:rowOff>
         </xdr:to>
@@ -5269,7 +5269,7 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>819150</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>9525</xdr:rowOff>
+          <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -6323,7 +6323,7 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>847725</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>114300</xdr:rowOff>
+          <xdr:rowOff>104775</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -6908,7 +6908,7 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>838200</xdr:colOff>
           <xdr:row>5</xdr:row>
-          <xdr:rowOff>114300</xdr:rowOff>
+          <xdr:rowOff>104775</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -7027,7 +7027,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>19050</xdr:colOff>
+          <xdr:colOff>9525</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>114300</xdr:rowOff>
         </xdr:to>
@@ -8083,7 +8083,7 @@
           <xdr:col>0</xdr:col>
           <xdr:colOff>666750</xdr:colOff>
           <xdr:row>6</xdr:row>
-          <xdr:rowOff>47625</xdr:rowOff>
+          <xdr:rowOff>38100</xdr:rowOff>
         </xdr:to>
         <xdr:sp macro="" textlink="">
           <xdr:nvSpPr>
@@ -8144,7 +8144,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>1933575</xdr:colOff>
+          <xdr:colOff>1924050</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:to>
@@ -8323,7 +8323,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>1933575</xdr:colOff>
+          <xdr:colOff>1924050</xdr:colOff>
           <xdr:row>4</xdr:row>
           <xdr:rowOff>152400</xdr:rowOff>
         </xdr:to>
@@ -8502,7 +8502,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>1933575</xdr:colOff>
+          <xdr:colOff>1924050</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -8918,7 +8918,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:to>
@@ -9213,7 +9213,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>3</xdr:col>
-          <xdr:colOff>9525</xdr:colOff>
+          <xdr:colOff>0</xdr:colOff>
           <xdr:row>3</xdr:row>
           <xdr:rowOff>47625</xdr:rowOff>
         </xdr:to>
@@ -9450,7 +9450,7 @@
         </xdr:from>
         <xdr:to>
           <xdr:col>4</xdr:col>
-          <xdr:colOff>1933575</xdr:colOff>
+          <xdr:colOff>1924050</xdr:colOff>
           <xdr:row>5</xdr:row>
           <xdr:rowOff>0</xdr:rowOff>
         </xdr:to>
@@ -10252,52 +10252,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="12289" r:id="rId4" name="cmdUpdate">
-          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId5">
+        <control shapeId="12300" r:id="rId4" name="optMultiRegionCommon">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
+                <xdr:colOff>47625</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>238125</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
+                <xdr:colOff>552450</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="12289" r:id="rId4" name="cmdUpdate"/>
+        <control shapeId="12300" r:id="rId4" name="optMultiRegionCommon"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="12291" r:id="rId6" name="cmdAddNewAnswerSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+        <control shapeId="12299" r:id="rId6" name="optMultiRegionNotCommon">
+          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:colOff>57150</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>228600</xdr:colOff>
-                <xdr:row>28</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
+                <xdr:colOff>571500</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="12291" r:id="rId6" name="cmdAddNewAnswerSheet"/>
+        <control shapeId="12299" r:id="rId6" name="optMultiRegionNotCommon"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10327,52 +10327,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="12299" r:id="rId10" name="optMultiRegionNotCommon">
-          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId11">
+        <control shapeId="12291" r:id="rId10" name="cmdAddNewAnswerSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>57150</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>571500</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
+                <xdr:colOff>228600</xdr:colOff>
+                <xdr:row>28</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="12299" r:id="rId10" name="optMultiRegionNotCommon"/>
+        <control shapeId="12291" r:id="rId10" name="cmdAddNewAnswerSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="12300" r:id="rId12" name="optMultiRegionCommon">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+        <control shapeId="12289" r:id="rId12" name="cmdUpdate">
+          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>47625</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>552450</xdr:colOff>
-                <xdr:row>21</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:colOff>238125</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="12300" r:id="rId12" name="optMultiRegionCommon"/>
+        <control shapeId="12289" r:id="rId12" name="cmdUpdate"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -10448,18 +10448,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="101377" r:id="rId4" name="cmdConstraintSets">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
+        <control shapeId="101379" r:id="rId4" name="cmdConstraintUnit">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
+                <xdr:col>3</xdr:col>
                 <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>571500</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>28575</xdr:rowOff>
               </to>
@@ -10468,7 +10468,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="101377" r:id="rId4" name="cmdConstraintSets"/>
+        <control shapeId="101379" r:id="rId4" name="cmdConstraintUnit"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10498,18 +10498,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="101379" r:id="rId8" name="cmdConstraintUnit">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+        <control shapeId="101377" r:id="rId8" name="cmdConstraintSets">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
+                <xdr:col>4</xdr:col>
                 <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>571500</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>28575</xdr:rowOff>
               </to>
@@ -10518,7 +10518,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="101379" r:id="rId8" name="cmdConstraintUnit"/>
+        <control shapeId="101377" r:id="rId8" name="cmdConstraintSets"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -10575,44 +10575,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="90116" r:id="rId4" name="cmdCheckCommDataSheet">
+        <control shapeId="90118" r:id="rId4" name="cmdAddParamQualifier2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="90116" r:id="rId4" name="cmdCheckCommDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="90115" r:id="rId6" name="cmdAddParamQualifier1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>5</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>5</xdr:row>
+                <xdr:row>6</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
@@ -10620,7 +10595,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="90115" r:id="rId6" name="cmdAddParamQualifier1"/>
+        <control shapeId="90118" r:id="rId4" name="cmdAddParamQualifier2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="90113" r:id="rId6" name="cmdAddParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="90113" r:id="rId6" name="cmdAddParameter"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10650,44 +10650,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="90113" r:id="rId10" name="cmdAddParameter">
+        <control shapeId="90115" r:id="rId10" name="cmdAddParamQualifier1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="90113" r:id="rId10" name="cmdAddParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="90118" r:id="rId12" name="cmdAddParamQualifier2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>6</xdr:row>
+                <xdr:row>5</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
@@ -10695,7 +10670,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="90118" r:id="rId12" name="cmdAddParamQualifier2"/>
+        <control shapeId="90115" r:id="rId10" name="cmdAddParamQualifier1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="90116" r:id="rId12" name="cmdCheckCommDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="90116" r:id="rId12" name="cmdCheckCommDataSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -10879,52 +10879,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="126981" r:id="rId4" name="cmdAddParamQualifier2">
+        <control shapeId="126977" r:id="rId4" name="cmdAddParameter">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="126981" r:id="rId4" name="cmdAddParamQualifier2"/>
+        <control shapeId="126977" r:id="rId4" name="cmdAddParameter"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="126980" r:id="rId6" name="cmdCheckCommDataSheet">
+        <control shapeId="126978" r:id="rId6" name="cmdCommNameAndDesc">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="126980" r:id="rId6" name="cmdCheckCommDataSheet"/>
+        <control shapeId="126978" r:id="rId6" name="cmdCommNameAndDesc"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -10954,52 +10954,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="126978" r:id="rId10" name="cmdCommNameAndDesc">
+        <control shapeId="126980" r:id="rId10" name="cmdCheckCommDataSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="126978" r:id="rId10" name="cmdCommNameAndDesc"/>
+        <control shapeId="126980" r:id="rId10" name="cmdCheckCommDataSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="126977" r:id="rId12" name="cmdAddParameter">
+        <control shapeId="126981" r:id="rId12" name="cmdAddParamQualifier2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="126977" r:id="rId12" name="cmdAddParameter"/>
+        <control shapeId="126981" r:id="rId12" name="cmdAddParamQualifier2"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -11377,18 +11377,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="128003" r:id="rId4" name="cmdProcUnits">
+        <control shapeId="128001" r:id="rId4" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>647700</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1924050</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -11397,7 +11397,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="128003" r:id="rId4" name="cmdProcUnits"/>
+        <control shapeId="128001" r:id="rId4" name="cmdSpecifySets"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -11427,18 +11427,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="128001" r:id="rId8" name="cmdSpecifySets">
+        <control shapeId="128003" r:id="rId8" name="cmdProcUnits">
           <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1924050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>647700</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -11447,7 +11447,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="128001" r:id="rId8" name="cmdSpecifySets"/>
+        <control shapeId="128003" r:id="rId8" name="cmdProcUnits"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -11528,18 +11528,43 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="113665" r:id="rId4" name="cmdTechNameAndDesc">
+        <control shapeId="113672" r:id="rId4" name="cmdAddParamQualifier2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="113672" r:id="rId4" name="cmdAddParamQualifier2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="113670" r:id="rId6" name="cmdCheckTechDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>1</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>1304925</xdr:colOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>209550</xdr:rowOff>
               </to>
@@ -11548,57 +11573,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="113665" r:id="rId4" name="cmdTechNameAndDesc"/>
+        <control shapeId="113670" r:id="rId6" name="cmdCheckTechDataSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="113666" r:id="rId6" name="cmdCommIN">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+        <control shapeId="113669" r:id="rId8" name="cmdAddParamQualifier1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>209550</xdr:rowOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="113666" r:id="rId6" name="cmdCommIN"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="113667" r:id="rId8" name="cmdCommOUT">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>619125</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>209550</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="113667" r:id="rId8" name="cmdCommOUT"/>
+        <control shapeId="113669" r:id="rId8" name="cmdAddParamQualifier1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -11628,43 +11628,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="113669" r:id="rId12" name="cmdAddParamQualifier1">
+        <control shapeId="113667" r:id="rId12" name="cmdCommOUT">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="113669" r:id="rId12" name="cmdAddParamQualifier1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="113670" r:id="rId14" name="cmdCheckTechDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
                 <xdr:row>1</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>619125</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>209550</xdr:rowOff>
               </to>
@@ -11673,32 +11648,57 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="113670" r:id="rId14" name="cmdCheckTechDataSheet"/>
+        <control shapeId="113667" r:id="rId12" name="cmdCommOUT"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="113672" r:id="rId16" name="cmdAddParamQualifier2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+        <control shapeId="113666" r:id="rId14" name="cmdCommIN">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>209550</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="113672" r:id="rId16" name="cmdAddParamQualifier2"/>
+        <control shapeId="113666" r:id="rId14" name="cmdCommIN"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="113665" r:id="rId16" name="cmdTechNameAndDesc">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>1304925</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>209550</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="113665" r:id="rId16" name="cmdTechNameAndDesc"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -12291,43 +12291,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="206855" r:id="rId4" name="cmdAddParamQualifier2">
+        <control shapeId="206849" r:id="rId4" name="cmdTechNameAndDesc">
           <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>647700</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="206855" r:id="rId4" name="cmdAddParamQualifier2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="206854" r:id="rId6" name="cmdCheckTechDataSheet">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
                 <xdr:row>1</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>647700</xdr:colOff>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>638175</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>190500</xdr:rowOff>
               </to>
@@ -12336,32 +12311,57 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="206854" r:id="rId6" name="cmdCheckTechDataSheet"/>
+        <control shapeId="206849" r:id="rId4" name="cmdTechNameAndDesc"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="206853" r:id="rId8" name="cmdAddParamQualifier1">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId9">
+        <control shapeId="206850" r:id="rId6" name="cmdCommIN">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>647700</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>609600</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="206853" r:id="rId8" name="cmdAddParamQualifier1"/>
+        <control shapeId="206850" r:id="rId6" name="cmdCommIN"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="206851" r:id="rId8" name="cmdCommOUT">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>609600</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="206851" r:id="rId8" name="cmdCommOUT"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -12391,18 +12391,43 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="206851" r:id="rId12" name="cmdCommOUT">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+        <control shapeId="206853" r:id="rId12" name="cmdAddParamQualifier1">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>647700</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="206853" r:id="rId12" name="cmdAddParamQualifier1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="206854" r:id="rId14" name="cmdCheckTechDataSheet">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>1</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>609600</xdr:colOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>647700</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>190500</xdr:rowOff>
               </to>
@@ -12411,57 +12436,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="206851" r:id="rId12" name="cmdCommOUT"/>
+        <control shapeId="206854" r:id="rId14" name="cmdCheckTechDataSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="206850" r:id="rId14" name="cmdCommIN">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+        <control shapeId="206855" r:id="rId16" name="cmdAddParamQualifier2">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId17">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>609600</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>647700</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="206850" r:id="rId14" name="cmdCommIN"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="206849" r:id="rId16" name="cmdTechNameAndDesc">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>638175</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="206849" r:id="rId16" name="cmdTechNameAndDesc"/>
+        <control shapeId="206855" r:id="rId16" name="cmdAddParamQualifier2"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -12739,18 +12739,43 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="233473" r:id="rId4" name="cmdTechNameAndDesc">
+        <control shapeId="233479" r:id="rId4" name="cmdAddParamQualifier2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>647700</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="233479" r:id="rId4" name="cmdAddParamQualifier2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="233478" r:id="rId6" name="cmdCheckTechDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>1</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>638175</xdr:colOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>647700</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>190500</xdr:rowOff>
               </to>
@@ -12759,57 +12784,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="233473" r:id="rId4" name="cmdTechNameAndDesc"/>
+        <control shapeId="233478" r:id="rId6" name="cmdCheckTechDataSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="233474" r:id="rId6" name="cmdCommIN">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+        <control shapeId="233477" r:id="rId8" name="cmdAddParamQualifier1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>609600</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>647700</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="233474" r:id="rId6" name="cmdCommIN"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="233475" r:id="rId8" name="cmdCommOUT">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>609600</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="233475" r:id="rId8" name="cmdCommOUT"/>
+        <control shapeId="233477" r:id="rId8" name="cmdAddParamQualifier1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -12839,43 +12839,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="233477" r:id="rId12" name="cmdAddParamQualifier1">
+        <control shapeId="233475" r:id="rId12" name="cmdCommOUT">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>647700</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="233477" r:id="rId12" name="cmdAddParamQualifier1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="233478" r:id="rId14" name="cmdCheckTechDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
                 <xdr:row>1</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>647700</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>609600</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>190500</xdr:rowOff>
               </to>
@@ -12884,32 +12859,57 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="233478" r:id="rId14" name="cmdCheckTechDataSheet"/>
+        <control shapeId="233475" r:id="rId12" name="cmdCommOUT"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="233479" r:id="rId16" name="cmdAddParamQualifier2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+        <control shapeId="233474" r:id="rId14" name="cmdCommIN">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>647700</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>609600</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="233479" r:id="rId16" name="cmdAddParamQualifier2"/>
+        <control shapeId="233474" r:id="rId14" name="cmdCommIN"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="233473" r:id="rId16" name="cmdTechNameAndDesc">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>638175</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="233473" r:id="rId16" name="cmdTechNameAndDesc"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -14589,8 +14589,183 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="102401" r:id="rId4" name="cmdConstrNameAndDesc">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
+        <control shapeId="102409" r:id="rId4" name="cmdAddParamQualifier2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>819150</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102409" r:id="rId4" name="cmdAddParamQualifier2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102408" r:id="rId6" name="cmdTimeSlice">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102408" r:id="rId6" name="cmdTimeSlice"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102407" r:id="rId8" name="cmdCommName">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102407" r:id="rId8" name="cmdCommName"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102405" r:id="rId10" name="cmdAddParamQualifier1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>819150</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102405" r:id="rId10" name="cmdAddParamQualifier1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102404" r:id="rId12" name="cmdCheckConstrDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102404" r:id="rId12" name="cmdCheckConstrDataSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102403" r:id="rId14" name="cmdAddParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>819150</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102403" r:id="rId14" name="cmdAddParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102402" r:id="rId16" name="cmdProcName">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102402" r:id="rId16" name="cmdProcName"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102401" r:id="rId18" name="cmdConstrNameAndDesc">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId19">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
@@ -14609,182 +14784,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="102401" r:id="rId4" name="cmdConstrNameAndDesc"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102402" r:id="rId6" name="cmdProcName">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102402" r:id="rId6" name="cmdProcName"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102403" r:id="rId8" name="cmdAddParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>819150</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102403" r:id="rId8" name="cmdAddParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102404" r:id="rId10" name="cmdCheckConstrDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102404" r:id="rId10" name="cmdCheckConstrDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102405" r:id="rId12" name="cmdAddParamQualifier1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>819150</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102405" r:id="rId12" name="cmdAddParamQualifier1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102407" r:id="rId14" name="cmdCommName">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102407" r:id="rId14" name="cmdCommName"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102408" r:id="rId16" name="cmdTimeSlice">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102408" r:id="rId16" name="cmdTimeSlice"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102409" r:id="rId18" name="cmdAddParamQualifier2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>819150</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102409" r:id="rId18" name="cmdAddParamQualifier2"/>
+        <control shapeId="102401" r:id="rId18" name="cmdConstrNameAndDesc"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -14933,8 +14933,83 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="55297" r:id="rId4" name="cmdCheckItemsSheet">
+        <control shapeId="55300" r:id="rId4" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="55300" r:id="rId4" name="cmdSpecifySets"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="55299" r:id="rId6" name="cmdSpecifyUnits">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="55299" r:id="rId6" name="cmdSpecifyUnits"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="55298" r:id="rId8" name="cmdSpecifyComponent">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>152400</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="55298" r:id="rId8" name="cmdSpecifyComponent"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="55297" r:id="rId10" name="cmdCheckItemsSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -14953,82 +15028,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="55297" r:id="rId4" name="cmdCheckItemsSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="55298" r:id="rId6" name="cmdSpecifyComponent">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>152400</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="55298" r:id="rId6" name="cmdSpecifyComponent"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="55299" r:id="rId8" name="cmdSpecifyUnits">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="55299" r:id="rId8" name="cmdSpecifyUnits"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="55300" r:id="rId10" name="cmdSpecifySets">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="55300" r:id="rId10" name="cmdSpecifySets"/>
+        <control shapeId="55297" r:id="rId10" name="cmdCheckItemsSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -15102,8 +15102,233 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="57354" r:id="rId4" name="cmdPopulateDataYears">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+        <control shapeId="57353" r:id="rId4" name="cmdSpecifyIEOptcode">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57353" r:id="rId4" name="cmdSpecifyIEOptcode"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57352" r:id="rId6" name="cmdSpecifyArg6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57352" r:id="rId6" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57351" r:id="rId8" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57351" r:id="rId8" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57350" r:id="rId10" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57350" r:id="rId10" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57349" r:id="rId12" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57349" r:id="rId12" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57348" r:id="rId14" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57348" r:id="rId14" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57347" r:id="rId16" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57347" r:id="rId16" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57346" r:id="rId18" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57346" r:id="rId18" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57345" r:id="rId20" name="cmdCheckTSDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57345" r:id="rId20" name="cmdCheckTSDataSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57354" r:id="rId22" name="cmdPopulateDataYears">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -15122,232 +15347,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="57354" r:id="rId4" name="cmdPopulateDataYears"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57345" r:id="rId6" name="cmdCheckTSDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57345" r:id="rId6" name="cmdCheckTSDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57346" r:id="rId8" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57346" r:id="rId8" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57347" r:id="rId10" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57347" r:id="rId10" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57348" r:id="rId12" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57348" r:id="rId12" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57349" r:id="rId14" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57349" r:id="rId14" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57350" r:id="rId16" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57350" r:id="rId16" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57351" r:id="rId18" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57351" r:id="rId18" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57352" r:id="rId20" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57352" r:id="rId20" name="cmdSpecifyArg6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57353" r:id="rId22" name="cmdSpecifyIEOptcode">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId23">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57353" r:id="rId22" name="cmdSpecifyIEOptcode"/>
+        <control shapeId="57354" r:id="rId22" name="cmdPopulateDataYears"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -15411,8 +15411,183 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="58369" r:id="rId4" name="cmdCheckTIDDataSheet">
+        <control shapeId="58376" r:id="rId4" name="cmdSpecifyArg6">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58376" r:id="rId4" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58375" r:id="rId6" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58375" r:id="rId6" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58374" r:id="rId8" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58374" r:id="rId8" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58373" r:id="rId10" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58373" r:id="rId10" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58372" r:id="rId12" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58372" r:id="rId12" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58371" r:id="rId14" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58371" r:id="rId14" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58370" r:id="rId16" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58370" r:id="rId16" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58369" r:id="rId18" name="cmdCheckTIDDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -15431,182 +15606,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="58369" r:id="rId4" name="cmdCheckTIDDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58370" r:id="rId6" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58370" r:id="rId6" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58371" r:id="rId8" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58371" r:id="rId8" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58372" r:id="rId10" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58372" r:id="rId10" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58373" r:id="rId12" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58373" r:id="rId12" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58374" r:id="rId14" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58374" r:id="rId14" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58375" r:id="rId16" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58375" r:id="rId16" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58376" r:id="rId18" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58376" r:id="rId18" name="cmdSpecifyArg6"/>
+        <control shapeId="58369" r:id="rId18" name="cmdCheckTIDDataSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -15681,8 +15681,233 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="59402" r:id="rId3" name="cmdPopulateDataYears">
+        <control shapeId="59401" r:id="rId3" name="cmdSpecifyIEOptcode">
           <controlPr defaultSize="0" autoLine="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>476250</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59401" r:id="rId3" name="cmdSpecifyIEOptcode"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59400" r:id="rId5" name="cmdSpecifyArg6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId6">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59400" r:id="rId5" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59399" r:id="rId7" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59399" r:id="rId7" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59398" r:id="rId9" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59398" r:id="rId9" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59397" r:id="rId11" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59397" r:id="rId11" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59396" r:id="rId13" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59396" r:id="rId13" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59395" r:id="rId15" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59395" r:id="rId15" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59394" r:id="rId17" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59394" r:id="rId17" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59393" r:id="rId19" name="cmdCheckTSandTIDDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId20">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>38100</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>857250</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>57150</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59393" r:id="rId19" name="cmdCheckTSandTIDDataSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59402" r:id="rId21" name="cmdPopulateDataYears">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -15701,232 +15926,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="59402" r:id="rId3" name="cmdPopulateDataYears"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59393" r:id="rId5" name="cmdCheckTSandTIDDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId6">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>38100</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>857250</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59393" r:id="rId5" name="cmdCheckTSandTIDDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59394" r:id="rId7" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59394" r:id="rId7" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59395" r:id="rId9" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59395" r:id="rId9" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59396" r:id="rId11" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59396" r:id="rId11" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59397" r:id="rId13" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59397" r:id="rId13" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59398" r:id="rId15" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59398" r:id="rId15" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59399" r:id="rId17" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59399" r:id="rId17" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59400" r:id="rId19" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId20">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59400" r:id="rId19" name="cmdSpecifyArg6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59401" r:id="rId21" name="cmdSpecifyIEOptcode">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>476250</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59401" r:id="rId21" name="cmdSpecifyIEOptcode"/>
+        <control shapeId="59402" r:id="rId21" name="cmdPopulateDataYears"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -16013,8 +16013,233 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="60427" r:id="rId3" name="cmdPopulateDataYears">
+        <control shapeId="60426" r:id="rId3" name="cmdCheckTSTradeSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>838200</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60426" r:id="rId3" name="cmdCheckTSTradeSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60425" r:id="rId5" name="cmdSpecifyIEOptcode">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId6">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60425" r:id="rId5" name="cmdSpecifyIEOptcode"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60424" r:id="rId7" name="cmdSpecifyArg6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60424" r:id="rId7" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60423" r:id="rId9" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60423" r:id="rId9" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60422" r:id="rId11" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60422" r:id="rId11" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60421" r:id="rId13" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60421" r:id="rId13" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60420" r:id="rId15" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60420" r:id="rId15" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60419" r:id="rId17" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60419" r:id="rId17" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60418" r:id="rId19" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId20">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60418" r:id="rId19" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60427" r:id="rId21" name="cmdPopulateDataYears">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -16033,232 +16258,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="60427" r:id="rId3" name="cmdPopulateDataYears"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60418" r:id="rId5" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId6">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60418" r:id="rId5" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60419" r:id="rId7" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60419" r:id="rId7" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60420" r:id="rId9" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60420" r:id="rId9" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60421" r:id="rId11" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60421" r:id="rId11" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60422" r:id="rId13" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60422" r:id="rId13" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60423" r:id="rId15" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60423" r:id="rId15" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60424" r:id="rId17" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60424" r:id="rId17" name="cmdSpecifyArg6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60425" r:id="rId19" name="cmdSpecifyIEOptcode">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId20">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>10</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60425" r:id="rId19" name="cmdSpecifyIEOptcode"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60426" r:id="rId21" name="cmdCheckTSTradeSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>838200</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60426" r:id="rId21" name="cmdCheckTSTradeSheet"/>
+        <control shapeId="60427" r:id="rId21" name="cmdPopulateDataYears"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -16335,8 +16335,183 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="61442" r:id="rId4" name="cmdCheckTIDTradeSheet">
+        <control shapeId="61449" r:id="rId4" name="cmdSpecifyArg6">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61449" r:id="rId4" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61448" r:id="rId6" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61448" r:id="rId6" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61447" r:id="rId8" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61447" r:id="rId8" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61446" r:id="rId10" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61446" r:id="rId10" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61445" r:id="rId12" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61445" r:id="rId12" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61444" r:id="rId14" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61444" r:id="rId14" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61443" r:id="rId16" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61443" r:id="rId16" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61442" r:id="rId18" name="cmdCheckTIDTradeSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -16355,182 +16530,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="61442" r:id="rId4" name="cmdCheckTIDTradeSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61443" r:id="rId6" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61443" r:id="rId6" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61444" r:id="rId8" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61444" r:id="rId8" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61445" r:id="rId10" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61445" r:id="rId10" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61446" r:id="rId12" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61446" r:id="rId12" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61447" r:id="rId14" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61447" r:id="rId14" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61448" r:id="rId16" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61448" r:id="rId16" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61449" r:id="rId18" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61449" r:id="rId18" name="cmdSpecifyArg6"/>
+        <control shapeId="61442" r:id="rId18" name="cmdCheckTIDTradeSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -16616,8 +16616,233 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="62475" r:id="rId4" name="cmdPopulateDataYears">
+        <control shapeId="62474" r:id="rId4" name="cmdSpecifyIEOptcode">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62474" r:id="rId4" name="cmdSpecifyIEOptcode"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62473" r:id="rId6" name="cmdSpecifyArg6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62473" r:id="rId6" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62472" r:id="rId8" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62472" r:id="rId8" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62471" r:id="rId10" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62471" r:id="rId10" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62470" r:id="rId12" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62470" r:id="rId12" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62469" r:id="rId14" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62469" r:id="rId14" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62468" r:id="rId16" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62468" r:id="rId16" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62467" r:id="rId18" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62467" r:id="rId18" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62466" r:id="rId20" name="cmdCheckTSandTIDTradeSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62466" r:id="rId20" name="cmdCheckTSandTIDTradeSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62475" r:id="rId22" name="cmdPopulateDataYears">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -16636,232 +16861,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="62475" r:id="rId4" name="cmdPopulateDataYears"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62466" r:id="rId6" name="cmdCheckTSandTIDTradeSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62466" r:id="rId6" name="cmdCheckTSandTIDTradeSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62467" r:id="rId8" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62467" r:id="rId8" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62468" r:id="rId10" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62468" r:id="rId10" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62469" r:id="rId12" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62469" r:id="rId12" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62470" r:id="rId14" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62470" r:id="rId14" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62471" r:id="rId16" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62471" r:id="rId16" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62472" r:id="rId18" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62472" r:id="rId18" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62473" r:id="rId20" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62473" r:id="rId20" name="cmdSpecifyArg6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62474" r:id="rId22" name="cmdSpecifyIEOptcode">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>10</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62474" r:id="rId22" name="cmdSpecifyIEOptcode"/>
+        <control shapeId="62475" r:id="rId22" name="cmdPopulateDataYears"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -19862,8 +19862,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="63489" r:id="rId4" name="cmdCheckRegionsSheet">
+        <control shapeId="63490" r:id="rId4" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="63490" r:id="rId4" name="cmdSpecifySets"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="63489" r:id="rId6" name="cmdCheckRegionsSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -19882,32 +19907,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="63489" r:id="rId4" name="cmdCheckRegionsSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="63490" r:id="rId6" name="cmdSpecifySets">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="63490" r:id="rId6" name="cmdSpecifySets"/>
+        <control shapeId="63489" r:id="rId6" name="cmdCheckRegionsSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -19968,18 +19968,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="71681" r:id="rId4" name="cmdSpecifySets">
+        <control shapeId="71683" r:id="rId4" name="cmdCommUnit">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1924050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>676275</xdr:colOff>
                 <xdr:row>4</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>
@@ -19988,7 +19988,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="71681" r:id="rId4" name="cmdSpecifySets"/>
+        <control shapeId="71683" r:id="rId4" name="cmdCommUnit"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -20018,18 +20018,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="71683" r:id="rId8" name="cmdCommUnit">
+        <control shapeId="71681" r:id="rId8" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>676275</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1924050</xdr:colOff>
                 <xdr:row>4</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>
@@ -20038,7 +20038,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="71683" r:id="rId8" name="cmdCommUnit"/>
+        <control shapeId="71681" r:id="rId8" name="cmdSpecifySets"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -20199,18 +20199,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="125955" r:id="rId4" name="cmdCommUnit">
+        <control shapeId="125953" r:id="rId4" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>676275</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1924050</xdr:colOff>
                 <xdr:row>4</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>
@@ -20219,7 +20219,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="125955" r:id="rId4" name="cmdCommUnit"/>
+        <control shapeId="125953" r:id="rId4" name="cmdSpecifySets"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -20249,18 +20249,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="125953" r:id="rId8" name="cmdSpecifySets">
+        <control shapeId="125955" r:id="rId8" name="cmdCommUnit">
           <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1924050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>676275</xdr:colOff>
                 <xdr:row>4</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>
@@ -20269,7 +20269,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="125953" r:id="rId8" name="cmdSpecifySets"/>
+        <control shapeId="125955" r:id="rId8" name="cmdCommUnit"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -20342,18 +20342,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="80899" r:id="rId4" name="cmdProcUnits">
+        <control shapeId="80897" r:id="rId4" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>647700</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1924050</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -20362,7 +20362,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="80899" r:id="rId4" name="cmdProcUnits"/>
+        <control shapeId="80897" r:id="rId4" name="cmdSpecifySets"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -20392,18 +20392,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="80897" r:id="rId8" name="cmdSpecifySets">
+        <control shapeId="80899" r:id="rId8" name="cmdProcUnits">
           <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1924050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>647700</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -20412,7 +20412,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="80897" r:id="rId8" name="cmdSpecifySets"/>
+        <control shapeId="80899" r:id="rId8" name="cmdProcUnits"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
Working across scenarios - pre CCS fixes
</commit_message>
<xml_diff>
--- a/SATIM/DataSpreadsheets/TCH_GRNEXP.xlsx
+++ b/SATIM/DataSpreadsheets/TCH_GRNEXP.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24430"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24527"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE\SATIM\DataSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BC72EDD0-4B40-4953-A909-01D7FDA2F327}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5EAC687-D2BC-4ACC-ABFA-6AE3AE1797E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="15" yWindow="15" windowWidth="28770" windowHeight="15570" tabRatio="796" activeTab="17" xr2:uid="{E4E4DEB2-CFB1-442C-9FC5-D51D154627BD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="796" activeTab="17" xr2:uid="{E4E4DEB2-CFB1-442C-9FC5-D51D154627BD}"/>
   </bookViews>
   <sheets>
     <sheet name="ANSv2-692-Home" sheetId="9" r:id="rId1"/>
@@ -2773,7 +2773,7 @@
 </file>
 
 <file path=xl/activeX/activeX1.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D50-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX10.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2905,7 +2905,7 @@
 </file>
 
 <file path=xl/activeX/activeX2.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D50-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX20.xml><?xml version="1.0" encoding="utf-8"?>
@@ -2993,7 +2993,7 @@
 </file>
 
 <file path=xl/activeX/activeX4.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D50-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX40.xml><?xml version="1.0" encoding="utf-8"?>
@@ -3037,7 +3037,7 @@
 </file>
 
 <file path=xl/activeX/activeX5.xml><?xml version="1.0" encoding="utf-8"?>
-<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{8BD21D50-EC42-11CE-9E0D-00AA006002F3}" ax:persistence="persistStreamInit" r:id="rId1"/>
+<ax:ocx xmlns:ax="http://schemas.microsoft.com/office/2006/activeX" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" ax:classid="{D7053240-CE69-11CD-A777-00DD01143C57}" ax:persistence="persistStreamInit" r:id="rId1"/>
 </file>
 
 <file path=xl/activeX/activeX50.xml><?xml version="1.0" encoding="utf-8"?>
@@ -11153,52 +11153,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="12289" r:id="rId4" name="cmdUpdate">
-          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId5">
+        <control shapeId="12300" r:id="rId4" name="optMultiRegionCommon">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>7</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
+                <xdr:colOff>47625</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>238125</xdr:colOff>
-                <xdr:row>12</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
+                <xdr:colOff>552450</xdr:colOff>
+                <xdr:row>21</xdr:row>
+                <xdr:rowOff>142875</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="12289" r:id="rId4" name="cmdUpdate"/>
+        <control shapeId="12300" r:id="rId4" name="optMultiRegionCommon"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="12291" r:id="rId6" name="cmdAddNewAnswerSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+        <control shapeId="12299" r:id="rId6" name="optMultiRegionNotCommon">
+          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>24</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:colOff>57150</xdr:colOff>
+                <xdr:row>14</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>228600</xdr:colOff>
-                <xdr:row>28</xdr:row>
-                <xdr:rowOff>76200</xdr:rowOff>
+                <xdr:colOff>571500</xdr:colOff>
+                <xdr:row>17</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="12291" r:id="rId6" name="cmdAddNewAnswerSheet"/>
+        <control shapeId="12299" r:id="rId6" name="optMultiRegionNotCommon"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -11228,52 +11228,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="12299" r:id="rId10" name="optMultiRegionNotCommon">
-          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId11">
+        <control shapeId="12291" r:id="rId10" name="cmdAddNewAnswerSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>57150</xdr:colOff>
-                <xdr:row>14</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>24</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>571500</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
+                <xdr:colOff>228600</xdr:colOff>
+                <xdr:row>28</xdr:row>
+                <xdr:rowOff>76200</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="12299" r:id="rId10" name="optMultiRegionNotCommon"/>
+        <control shapeId="12291" r:id="rId10" name="cmdAddNewAnswerSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="12300" r:id="rId12" name="optMultiRegionCommon">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+        <control shapeId="12289" r:id="rId12" name="cmdUpdate">
+          <controlPr defaultSize="0" disabled="1" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>47625</xdr:colOff>
-                <xdr:row>17</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>7</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>3</xdr:col>
-                <xdr:colOff>552450</xdr:colOff>
-                <xdr:row>21</xdr:row>
-                <xdr:rowOff>142875</xdr:rowOff>
+                <xdr:colOff>238125</xdr:colOff>
+                <xdr:row>12</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="12300" r:id="rId12" name="optMultiRegionCommon"/>
+        <control shapeId="12289" r:id="rId12" name="cmdUpdate"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -11349,18 +11349,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="101377" r:id="rId4" name="cmdConstraintSets">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
+        <control shapeId="101379" r:id="rId4" name="cmdConstraintUnit">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
+                <xdr:col>3</xdr:col>
                 <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:rowOff>9525</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>571500</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>28575</xdr:rowOff>
               </to>
@@ -11369,7 +11369,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="101377" r:id="rId4" name="cmdConstraintSets"/>
+        <control shapeId="101379" r:id="rId4" name="cmdConstraintUnit"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -11399,18 +11399,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="101379" r:id="rId8" name="cmdConstraintUnit">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+        <control shapeId="101377" r:id="rId8" name="cmdConstraintSets">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
+                <xdr:col>4</xdr:col>
                 <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>571500</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>28575</xdr:rowOff>
               </to>
@@ -11419,7 +11419,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="101379" r:id="rId8" name="cmdConstraintUnit"/>
+        <control shapeId="101377" r:id="rId8" name="cmdConstraintSets"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -11476,44 +11476,19 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="90116" r:id="rId4" name="cmdCheckCommDataSheet">
+        <control shapeId="90118" r:id="rId4" name="cmdAddParamQualifier2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="90116" r:id="rId4" name="cmdCheckCommDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="90115" r:id="rId6" name="cmdAddParamQualifier1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
+                <xdr:row>5</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>5</xdr:row>
+                <xdr:row>6</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
@@ -11521,7 +11496,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="90115" r:id="rId6" name="cmdAddParamQualifier1"/>
+        <control shapeId="90118" r:id="rId4" name="cmdAddParamQualifier2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="90113" r:id="rId6" name="cmdAddParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="90113" r:id="rId6" name="cmdAddParameter"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -11551,44 +11551,19 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="90113" r:id="rId10" name="cmdAddParameter">
+        <control shapeId="90115" r:id="rId10" name="cmdAddParamQualifier1">
           <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
                 <xdr:row>4</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="90113" r:id="rId10" name="cmdAddParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="90118" r:id="rId12" name="cmdAddParamQualifier2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
                 <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>6</xdr:row>
+                <xdr:row>5</xdr:row>
                 <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
@@ -11596,7 +11571,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="90118" r:id="rId12" name="cmdAddParamQualifier2"/>
+        <control shapeId="90115" r:id="rId10" name="cmdAddParamQualifier1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="90116" r:id="rId12" name="cmdCheckCommDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="90116" r:id="rId12" name="cmdCheckCommDataSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -11780,52 +11780,52 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="126981" r:id="rId4" name="cmdAddParamQualifier2">
+        <control shapeId="126977" r:id="rId4" name="cmdAddParameter">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="126981" r:id="rId4" name="cmdAddParamQualifier2"/>
+        <control shapeId="126977" r:id="rId4" name="cmdAddParameter"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="126980" r:id="rId6" name="cmdCheckCommDataSheet">
+        <control shapeId="126978" r:id="rId6" name="cmdCommNameAndDesc">
           <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>123825</xdr:rowOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
+                <xdr:rowOff>47625</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="126980" r:id="rId6" name="cmdCheckCommDataSheet"/>
+        <control shapeId="126978" r:id="rId6" name="cmdCommNameAndDesc"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -11855,52 +11855,52 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="126978" r:id="rId10" name="cmdCommNameAndDesc">
+        <control shapeId="126980" r:id="rId10" name="cmdCheckCommDataSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>123825</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
                 <xdr:row>3</xdr:row>
-                <xdr:rowOff>47625</xdr:rowOff>
+                <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="126978" r:id="rId10" name="cmdCommNameAndDesc"/>
+        <control shapeId="126980" r:id="rId10" name="cmdCheckCommDataSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="126977" r:id="rId12" name="cmdAddParameter">
+        <control shapeId="126981" r:id="rId12" name="cmdAddParamQualifier2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
                 <xdr:col>0</xdr:col>
                 <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="126977" r:id="rId12" name="cmdAddParameter"/>
+        <control shapeId="126981" r:id="rId12" name="cmdAddParamQualifier2"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -12304,18 +12304,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="128003" r:id="rId4" name="cmdProcUnits">
+        <control shapeId="128001" r:id="rId4" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>647700</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1924050</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -12324,7 +12324,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="128003" r:id="rId4" name="cmdProcUnits"/>
+        <control shapeId="128001" r:id="rId4" name="cmdSpecifySets"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -12354,18 +12354,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="128001" r:id="rId8" name="cmdSpecifySets">
+        <control shapeId="128003" r:id="rId8" name="cmdProcUnits">
           <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1924050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>647700</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -12374,7 +12374,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="128001" r:id="rId8" name="cmdSpecifySets"/>
+        <control shapeId="128003" r:id="rId8" name="cmdProcUnits"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -12455,18 +12455,43 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="113665" r:id="rId4" name="cmdTechNameAndDesc">
+        <control shapeId="113672" r:id="rId4" name="cmdAddParamQualifier2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
                 <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="113672" r:id="rId4" name="cmdAddParamQualifier2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="113670" r:id="rId6" name="cmdCheckTechDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>1</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>1304925</xdr:colOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>209550</xdr:rowOff>
               </to>
@@ -12475,57 +12500,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="113665" r:id="rId4" name="cmdTechNameAndDesc"/>
+        <control shapeId="113670" r:id="rId6" name="cmdCheckTechDataSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="113666" r:id="rId6" name="cmdCommIN">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+        <control shapeId="113669" r:id="rId8" name="cmdAddParamQualifier1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>209550</xdr:rowOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="113666" r:id="rId6" name="cmdCommIN"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="113667" r:id="rId8" name="cmdCommOUT">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>619125</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>209550</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="113667" r:id="rId8" name="cmdCommOUT"/>
+        <control shapeId="113669" r:id="rId8" name="cmdAddParamQualifier1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -12555,43 +12555,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="113669" r:id="rId12" name="cmdAddParamQualifier1">
+        <control shapeId="113667" r:id="rId12" name="cmdCommOUT">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="113669" r:id="rId12" name="cmdAddParamQualifier1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="113670" r:id="rId14" name="cmdCheckTechDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
                 <xdr:row>1</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>619125</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>209550</xdr:rowOff>
               </to>
@@ -12600,32 +12575,57 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="113670" r:id="rId14" name="cmdCheckTechDataSheet"/>
+        <control shapeId="113667" r:id="rId12" name="cmdCommOUT"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="113672" r:id="rId16" name="cmdAddParamQualifier2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+        <control shapeId="113666" r:id="rId14" name="cmdCommIN">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>209550</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="113672" r:id="rId16" name="cmdAddParamQualifier2"/>
+        <control shapeId="113666" r:id="rId14" name="cmdCommIN"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="113665" r:id="rId16" name="cmdTechNameAndDesc">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>1304925</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>209550</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="113665" r:id="rId16" name="cmdTechNameAndDesc"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -12639,8 +12639,8 @@
   </sheetPr>
   <dimension ref="A1:AA15"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="AA9" sqref="AA9"/>
+    <sheetView topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="AA15" sqref="AA15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -13381,43 +13381,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="206855" r:id="rId4" name="cmdAddParamQualifier2">
+        <control shapeId="206849" r:id="rId4" name="cmdTechNameAndDesc">
           <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>647700</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="206855" r:id="rId4" name="cmdAddParamQualifier2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="206854" r:id="rId6" name="cmdCheckTechDataSheet">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
                 <xdr:row>1</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>647700</xdr:colOff>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>638175</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>190500</xdr:rowOff>
               </to>
@@ -13426,32 +13401,57 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="206854" r:id="rId6" name="cmdCheckTechDataSheet"/>
+        <control shapeId="206849" r:id="rId4" name="cmdTechNameAndDesc"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="206853" r:id="rId8" name="cmdAddParamQualifier1">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId9">
+        <control shapeId="206850" r:id="rId6" name="cmdCommIN">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>647700</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>609600</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="206853" r:id="rId8" name="cmdAddParamQualifier1"/>
+        <control shapeId="206850" r:id="rId6" name="cmdCommIN"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="206851" r:id="rId8" name="cmdCommOUT">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>609600</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="206851" r:id="rId8" name="cmdCommOUT"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -13481,18 +13481,43 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="206851" r:id="rId12" name="cmdCommOUT">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+        <control shapeId="206853" r:id="rId12" name="cmdAddParamQualifier1">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>647700</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="206853" r:id="rId12" name="cmdAddParamQualifier1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="206854" r:id="rId14" name="cmdCheckTechDataSheet">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>1</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>609600</xdr:colOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>647700</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>190500</xdr:rowOff>
               </to>
@@ -13501,57 +13526,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="206851" r:id="rId12" name="cmdCommOUT"/>
+        <control shapeId="206854" r:id="rId14" name="cmdCheckTechDataSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="206850" r:id="rId14" name="cmdCommIN">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+        <control shapeId="206855" r:id="rId16" name="cmdAddParamQualifier2">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId17">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>609600</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>647700</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="206850" r:id="rId14" name="cmdCommIN"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="206849" r:id="rId16" name="cmdTechNameAndDesc">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>638175</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="206849" r:id="rId16" name="cmdTechNameAndDesc"/>
+        <control shapeId="206855" r:id="rId16" name="cmdAddParamQualifier2"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -13827,18 +13827,43 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="233473" r:id="rId4" name="cmdTechNameAndDesc">
+        <control shapeId="233479" r:id="rId4" name="cmdAddParamQualifier2">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>647700</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="233479" r:id="rId4" name="cmdAddParamQualifier2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="233478" r:id="rId6" name="cmdCheckTechDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>1</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>638175</xdr:colOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>647700</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>190500</xdr:rowOff>
               </to>
@@ -13847,57 +13872,32 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="233473" r:id="rId4" name="cmdTechNameAndDesc"/>
+        <control shapeId="233478" r:id="rId6" name="cmdCheckTechDataSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="233474" r:id="rId6" name="cmdCommIN">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+        <control shapeId="233477" r:id="rId8" name="cmdAddParamQualifier1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>171450</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>609600</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>647700</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="233474" r:id="rId6" name="cmdCommIN"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="233475" r:id="rId8" name="cmdCommOUT">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>1</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>609600</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="233475" r:id="rId8" name="cmdCommOUT"/>
+        <control shapeId="233477" r:id="rId8" name="cmdAddParamQualifier1"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -13927,43 +13927,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="233477" r:id="rId12" name="cmdAddParamQualifier1">
+        <control shapeId="233475" r:id="rId12" name="cmdCommOUT">
           <controlPr defaultSize="0" autoLine="0" r:id="rId13">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>171450</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>647700</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="233477" r:id="rId12" name="cmdAddParamQualifier1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="233478" r:id="rId14" name="cmdCheckTechDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
                 <xdr:row>1</xdr:row>
                 <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>647700</xdr:colOff>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>609600</xdr:colOff>
                 <xdr:row>2</xdr:row>
                 <xdr:rowOff>190500</xdr:rowOff>
               </to>
@@ -13972,32 +13947,57 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="233478" r:id="rId14" name="cmdCheckTechDataSheet"/>
+        <control shapeId="233475" r:id="rId12" name="cmdCommOUT"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="233479" r:id="rId16" name="cmdAddParamQualifier2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+        <control shapeId="233474" r:id="rId14" name="cmdCommIN">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>647700</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>609600</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
               </to>
             </anchor>
           </controlPr>
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="233479" r:id="rId16" name="cmdAddParamQualifier2"/>
+        <control shapeId="233474" r:id="rId14" name="cmdCommIN"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="233473" r:id="rId16" name="cmdTechNameAndDesc">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>1</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>638175</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="233473" r:id="rId16" name="cmdTechNameAndDesc"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -14454,8 +14454,8 @@
   </sheetPr>
   <dimension ref="B2:AW53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="U1" workbookViewId="0">
-      <selection activeCell="AW26" sqref="AW26"/>
+    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+      <selection activeCell="W6" sqref="W6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -16767,8 +16767,183 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="102401" r:id="rId4" name="cmdConstrNameAndDesc">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
+        <control shapeId="102409" r:id="rId4" name="cmdAddParamQualifier2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>819150</xdr:colOff>
+                <xdr:row>6</xdr:row>
+                <xdr:rowOff>38100</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102409" r:id="rId4" name="cmdAddParamQualifier2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102408" r:id="rId6" name="cmdTimeSlice">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102408" r:id="rId6" name="cmdTimeSlice"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102407" r:id="rId8" name="cmdCommName">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102407" r:id="rId8" name="cmdCommName"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102405" r:id="rId10" name="cmdAddParamQualifier1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>819150</xdr:colOff>
+                <xdr:row>5</xdr:row>
+                <xdr:rowOff>28575</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102405" r:id="rId10" name="cmdAddParamQualifier1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102404" r:id="rId12" name="cmdCheckConstrDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102404" r:id="rId12" name="cmdCheckConstrDataSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102403" r:id="rId14" name="cmdAddParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>190500</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>819150</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>152400</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102403" r:id="rId14" name="cmdAddParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102402" r:id="rId16" name="cmdProcName">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>238125</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="102402" r:id="rId16" name="cmdProcName"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="102401" r:id="rId18" name="cmdConstrNameAndDesc">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId19">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>1</xdr:col>
@@ -16787,182 +16962,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="102401" r:id="rId4" name="cmdConstrNameAndDesc"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102402" r:id="rId6" name="cmdProcName">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102402" r:id="rId6" name="cmdProcName"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102403" r:id="rId8" name="cmdAddParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>190500</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>819150</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>152400</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102403" r:id="rId8" name="cmdAddParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102404" r:id="rId10" name="cmdCheckConstrDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102404" r:id="rId10" name="cmdCheckConstrDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102405" r:id="rId12" name="cmdAddParamQualifier1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>819150</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>28575</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102405" r:id="rId12" name="cmdAddParamQualifier1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102407" r:id="rId14" name="cmdCommName">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102407" r:id="rId14" name="cmdCommName"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102408" r:id="rId16" name="cmdTimeSlice">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>238125</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102408" r:id="rId16" name="cmdTimeSlice"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="102409" r:id="rId18" name="cmdAddParamQualifier2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>5</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>819150</xdr:colOff>
-                <xdr:row>6</xdr:row>
-                <xdr:rowOff>38100</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="102409" r:id="rId18" name="cmdAddParamQualifier2"/>
+        <control shapeId="102401" r:id="rId18" name="cmdConstrNameAndDesc"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -17111,8 +17111,83 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="55297" r:id="rId4" name="cmdCheckItemsSheet">
+        <control shapeId="55300" r:id="rId4" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="55300" r:id="rId4" name="cmdSpecifySets"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="55299" r:id="rId6" name="cmdSpecifyUnits">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="55299" r:id="rId6" name="cmdSpecifyUnits"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="55298" r:id="rId8" name="cmdSpecifyComponent">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>152400</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="55298" r:id="rId8" name="cmdSpecifyComponent"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="55297" r:id="rId10" name="cmdCheckItemsSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -17131,82 +17206,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="55297" r:id="rId4" name="cmdCheckItemsSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="55298" r:id="rId6" name="cmdSpecifyComponent">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>152400</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="55298" r:id="rId6" name="cmdSpecifyComponent"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="55299" r:id="rId8" name="cmdSpecifyUnits">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="55299" r:id="rId8" name="cmdSpecifyUnits"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="55300" r:id="rId10" name="cmdSpecifySets">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="55300" r:id="rId10" name="cmdSpecifySets"/>
+        <control shapeId="55297" r:id="rId10" name="cmdCheckItemsSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -17280,8 +17280,233 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="57354" r:id="rId4" name="cmdPopulateDataYears">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+        <control shapeId="57353" r:id="rId4" name="cmdSpecifyIEOptcode">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57353" r:id="rId4" name="cmdSpecifyIEOptcode"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57352" r:id="rId6" name="cmdSpecifyArg6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57352" r:id="rId6" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57351" r:id="rId8" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57351" r:id="rId8" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57350" r:id="rId10" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57350" r:id="rId10" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57349" r:id="rId12" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57349" r:id="rId12" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57348" r:id="rId14" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57348" r:id="rId14" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57347" r:id="rId16" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57347" r:id="rId16" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57346" r:id="rId18" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57346" r:id="rId18" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57345" r:id="rId20" name="cmdCheckTSDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="57345" r:id="rId20" name="cmdCheckTSDataSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="57354" r:id="rId22" name="cmdPopulateDataYears">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -17300,232 +17525,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="57354" r:id="rId4" name="cmdPopulateDataYears"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57345" r:id="rId6" name="cmdCheckTSDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57345" r:id="rId6" name="cmdCheckTSDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57346" r:id="rId8" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57346" r:id="rId8" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57347" r:id="rId10" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57347" r:id="rId10" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57348" r:id="rId12" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57348" r:id="rId12" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57349" r:id="rId14" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57349" r:id="rId14" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57350" r:id="rId16" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57350" r:id="rId16" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57351" r:id="rId18" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57351" r:id="rId18" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57352" r:id="rId20" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57352" r:id="rId20" name="cmdSpecifyArg6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="57353" r:id="rId22" name="cmdSpecifyIEOptcode">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId23">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="57353" r:id="rId22" name="cmdSpecifyIEOptcode"/>
+        <control shapeId="57354" r:id="rId22" name="cmdPopulateDataYears"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -17589,8 +17589,183 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="58369" r:id="rId4" name="cmdCheckTIDDataSheet">
+        <control shapeId="58376" r:id="rId4" name="cmdSpecifyArg6">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58376" r:id="rId4" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58375" r:id="rId6" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58375" r:id="rId6" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58374" r:id="rId8" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58374" r:id="rId8" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58373" r:id="rId10" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58373" r:id="rId10" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58372" r:id="rId12" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58372" r:id="rId12" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58371" r:id="rId14" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58371" r:id="rId14" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58370" r:id="rId16" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>95250</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="58370" r:id="rId16" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="58369" r:id="rId18" name="cmdCheckTIDDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -17609,182 +17784,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="58369" r:id="rId4" name="cmdCheckTIDDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58370" r:id="rId6" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58370" r:id="rId6" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58371" r:id="rId8" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58371" r:id="rId8" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58372" r:id="rId10" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58372" r:id="rId10" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58373" r:id="rId12" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58373" r:id="rId12" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58374" r:id="rId14" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58374" r:id="rId14" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58375" r:id="rId16" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58375" r:id="rId16" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="58376" r:id="rId18" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>95250</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="58376" r:id="rId18" name="cmdSpecifyArg6"/>
+        <control shapeId="58369" r:id="rId18" name="cmdCheckTIDDataSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -17859,8 +17859,233 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="59402" r:id="rId3" name="cmdPopulateDataYears">
+        <control shapeId="59401" r:id="rId3" name="cmdSpecifyIEOptcode">
           <controlPr defaultSize="0" autoLine="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>476250</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59401" r:id="rId3" name="cmdSpecifyIEOptcode"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59400" r:id="rId5" name="cmdSpecifyArg6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId6">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59400" r:id="rId5" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59399" r:id="rId7" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59399" r:id="rId7" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59398" r:id="rId9" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59398" r:id="rId9" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59397" r:id="rId11" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59397" r:id="rId11" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59396" r:id="rId13" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59396" r:id="rId13" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59395" r:id="rId15" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59395" r:id="rId15" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59394" r:id="rId17" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>1</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59394" r:id="rId17" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59393" r:id="rId19" name="cmdCheckTSandTIDDataSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId20">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>38100</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>857250</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>57150</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="59393" r:id="rId19" name="cmdCheckTSandTIDDataSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="59402" r:id="rId21" name="cmdPopulateDataYears">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -17879,232 +18104,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="59402" r:id="rId3" name="cmdPopulateDataYears"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59393" r:id="rId5" name="cmdCheckTSandTIDDataSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId6">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>38100</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>857250</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>57150</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59393" r:id="rId5" name="cmdCheckTSandTIDDataSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59394" r:id="rId7" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>1</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59394" r:id="rId7" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59395" r:id="rId9" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59395" r:id="rId9" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59396" r:id="rId11" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59396" r:id="rId11" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59397" r:id="rId13" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59397" r:id="rId13" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59398" r:id="rId15" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59398" r:id="rId15" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59399" r:id="rId17" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59399" r:id="rId17" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59400" r:id="rId19" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId20">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59400" r:id="rId19" name="cmdSpecifyArg6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="59401" r:id="rId21" name="cmdSpecifyIEOptcode">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>476250</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="59401" r:id="rId21" name="cmdSpecifyIEOptcode"/>
+        <control shapeId="59402" r:id="rId21" name="cmdPopulateDataYears"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -18191,8 +18191,233 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="60427" r:id="rId3" name="cmdPopulateDataYears">
+        <control shapeId="60426" r:id="rId3" name="cmdCheckTSTradeSheet">
           <controlPr defaultSize="0" autoLine="0" r:id="rId4">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>838200</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60426" r:id="rId3" name="cmdCheckTSTradeSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60425" r:id="rId5" name="cmdSpecifyIEOptcode">
+          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId6">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60425" r:id="rId5" name="cmdSpecifyIEOptcode"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60424" r:id="rId7" name="cmdSpecifyArg6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60424" r:id="rId7" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60423" r:id="rId9" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60423" r:id="rId9" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60422" r:id="rId11" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60422" r:id="rId11" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60421" r:id="rId13" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60421" r:id="rId13" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60420" r:id="rId15" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60420" r:id="rId15" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60419" r:id="rId17" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60419" r:id="rId17" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60418" r:id="rId19" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId20">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>104775</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="60418" r:id="rId19" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="60427" r:id="rId21" name="cmdPopulateDataYears">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -18211,232 +18436,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="60427" r:id="rId3" name="cmdPopulateDataYears"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60418" r:id="rId5" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId6">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60418" r:id="rId5" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60419" r:id="rId7" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId8">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60419" r:id="rId7" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60420" r:id="rId9" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId10">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60420" r:id="rId9" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60421" r:id="rId11" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId12">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60421" r:id="rId11" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60422" r:id="rId13" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId14">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60422" r:id="rId13" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60423" r:id="rId15" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId16">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60423" r:id="rId15" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60424" r:id="rId17" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId18">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>104775</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60424" r:id="rId17" name="cmdSpecifyArg6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60425" r:id="rId19" name="cmdSpecifyIEOptcode">
-          <controlPr defaultSize="0" autoLine="0" autoPict="0" r:id="rId20">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>10</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60425" r:id="rId19" name="cmdSpecifyIEOptcode"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="60426" r:id="rId21" name="cmdCheckTSTradeSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId22">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>838200</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="60426" r:id="rId21" name="cmdCheckTSTradeSheet"/>
+        <control shapeId="60427" r:id="rId21" name="cmdPopulateDataYears"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -18513,8 +18513,183 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="61442" r:id="rId4" name="cmdCheckTIDTradeSheet">
+        <control shapeId="61449" r:id="rId4" name="cmdSpecifyArg6">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61449" r:id="rId4" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61448" r:id="rId6" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61448" r:id="rId6" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61447" r:id="rId8" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61447" r:id="rId8" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61446" r:id="rId10" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61446" r:id="rId10" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61445" r:id="rId12" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61445" r:id="rId12" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61444" r:id="rId14" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61444" r:id="rId14" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61443" r:id="rId16" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>0</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="61443" r:id="rId16" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="61442" r:id="rId18" name="cmdCheckTIDTradeSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -18533,182 +18708,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="61442" r:id="rId4" name="cmdCheckTIDTradeSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61443" r:id="rId6" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61443" r:id="rId6" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61444" r:id="rId8" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>0</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61444" r:id="rId8" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61445" r:id="rId10" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61445" r:id="rId10" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61446" r:id="rId12" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61446" r:id="rId12" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61447" r:id="rId14" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61447" r:id="rId14" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61448" r:id="rId16" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61448" r:id="rId16" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="61449" r:id="rId18" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="61449" r:id="rId18" name="cmdSpecifyArg6"/>
+        <control shapeId="61442" r:id="rId18" name="cmdCheckTIDTradeSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -18794,8 +18794,233 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="62475" r:id="rId4" name="cmdPopulateDataYears">
+        <control shapeId="62474" r:id="rId4" name="cmdSpecifyIEOptcode">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>28575</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>10</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62474" r:id="rId4" name="cmdSpecifyIEOptcode"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62473" r:id="rId6" name="cmdSpecifyArg6">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>9</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62473" r:id="rId6" name="cmdSpecifyArg6"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62472" r:id="rId8" name="cmdSpecifyArg5">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>8</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62472" r:id="rId8" name="cmdSpecifyArg5"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62471" r:id="rId10" name="cmdSpecifyArg4">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>7</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62471" r:id="rId10" name="cmdSpecifyArg4"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62470" r:id="rId12" name="cmdSpecifyArg3">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>6</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62470" r:id="rId12" name="cmdSpecifyArg3"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62469" r:id="rId14" name="cmdSpecifyArg2">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>5</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62469" r:id="rId14" name="cmdSpecifyArg2"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62468" r:id="rId16" name="cmdSpecifyArg1">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62468" r:id="rId16" name="cmdSpecifyArg1"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62467" r:id="rId18" name="cmdSpecifyParameter">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>9525</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>85725</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62467" r:id="rId18" name="cmdSpecifyParameter"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62466" r:id="rId20" name="cmdCheckTSandTIDTradeSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>2</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>0</xdr:col>
+                <xdr:colOff>828675</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>0</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="62466" r:id="rId20" name="cmdCheckTSandTIDTradeSheet"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="62475" r:id="rId22" name="cmdPopulateDataYears">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -18814,232 +19039,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="62475" r:id="rId4" name="cmdPopulateDataYears"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62466" r:id="rId6" name="cmdCheckTSandTIDTradeSheet">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>2</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>0</xdr:col>
-                <xdr:colOff>828675</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>0</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62466" r:id="rId6" name="cmdCheckTSandTIDTradeSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62467" r:id="rId8" name="cmdSpecifyParameter">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId9">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62467" r:id="rId8" name="cmdSpecifyParameter"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62468" r:id="rId10" name="cmdSpecifyArg1">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId11">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62468" r:id="rId10" name="cmdSpecifyArg1"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62469" r:id="rId12" name="cmdSpecifyArg2">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId13">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62469" r:id="rId12" name="cmdSpecifyArg2"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62470" r:id="rId14" name="cmdSpecifyArg3">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId15">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>5</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62470" r:id="rId14" name="cmdSpecifyArg3"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62471" r:id="rId16" name="cmdSpecifyArg4">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId17">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>6</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62471" r:id="rId16" name="cmdSpecifyArg4"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62472" r:id="rId18" name="cmdSpecifyArg5">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId19">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>7</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62472" r:id="rId18" name="cmdSpecifyArg5"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62473" r:id="rId20" name="cmdSpecifyArg6">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId21">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>8</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62473" r:id="rId20" name="cmdSpecifyArg6"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="62474" r:id="rId22" name="cmdSpecifyIEOptcode">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId23">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>9</xdr:col>
-                <xdr:colOff>28575</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>9525</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>10</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>85725</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="62474" r:id="rId22" name="cmdSpecifyIEOptcode"/>
+        <control shapeId="62475" r:id="rId22" name="cmdPopulateDataYears"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -22355,8 +22355,33 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="63489" r:id="rId4" name="cmdCheckRegionsSheet">
+        <control shapeId="63490" r:id="rId4" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
+            <anchor moveWithCells="1">
+              <from>
+                <xdr:col>2</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>3</xdr:row>
+                <xdr:rowOff>19050</xdr:rowOff>
+              </from>
+              <to>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
+                <xdr:row>4</xdr:row>
+                <xdr:rowOff>114300</xdr:rowOff>
+              </to>
+            </anchor>
+          </controlPr>
+        </control>
+      </mc:Choice>
+      <mc:Fallback>
+        <control shapeId="63490" r:id="rId4" name="cmdSpecifySets"/>
+      </mc:Fallback>
+    </mc:AlternateContent>
+    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+      <mc:Choice Requires="x14">
+        <control shapeId="63489" r:id="rId6" name="cmdCheckRegionsSheet">
+          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
             <anchor moveWithCells="1">
               <from>
                 <xdr:col>0</xdr:col>
@@ -22375,32 +22400,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="63489" r:id="rId4" name="cmdCheckRegionsSheet"/>
-      </mc:Fallback>
-    </mc:AlternateContent>
-    <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-      <mc:Choice Requires="x14">
-        <control shapeId="63490" r:id="rId6" name="cmdSpecifySets">
-          <controlPr defaultSize="0" autoLine="0" r:id="rId7">
-            <anchor moveWithCells="1">
-              <from>
-                <xdr:col>2</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>3</xdr:row>
-                <xdr:rowOff>19050</xdr:rowOff>
-              </from>
-              <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
-                <xdr:row>4</xdr:row>
-                <xdr:rowOff>114300</xdr:rowOff>
-              </to>
-            </anchor>
-          </controlPr>
-        </control>
-      </mc:Choice>
-      <mc:Fallback>
-        <control shapeId="63490" r:id="rId6" name="cmdSpecifySets"/>
+        <control shapeId="63489" r:id="rId6" name="cmdCheckRegionsSheet"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -22461,18 +22461,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="71681" r:id="rId4" name="cmdSpecifySets">
+        <control shapeId="71683" r:id="rId4" name="cmdCommUnit">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1924050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>676275</xdr:colOff>
                 <xdr:row>4</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>
@@ -22481,7 +22481,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="71681" r:id="rId4" name="cmdSpecifySets"/>
+        <control shapeId="71683" r:id="rId4" name="cmdCommUnit"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -22511,18 +22511,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="71683" r:id="rId8" name="cmdCommUnit">
+        <control shapeId="71681" r:id="rId8" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>676275</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1924050</xdr:colOff>
                 <xdr:row>4</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>
@@ -22531,7 +22531,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="71683" r:id="rId8" name="cmdCommUnit"/>
+        <control shapeId="71681" r:id="rId8" name="cmdSpecifySets"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -22738,18 +22738,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="125955" r:id="rId4" name="cmdCommUnit">
+        <control shapeId="125953" r:id="rId4" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>676275</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1924050</xdr:colOff>
                 <xdr:row>4</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>
@@ -22758,7 +22758,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="125955" r:id="rId4" name="cmdCommUnit"/>
+        <control shapeId="125953" r:id="rId4" name="cmdSpecifySets"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -22788,18 +22788,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="125953" r:id="rId8" name="cmdSpecifySets">
+        <control shapeId="125955" r:id="rId8" name="cmdCommUnit">
           <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1924050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>676275</xdr:colOff>
                 <xdr:row>4</xdr:row>
                 <xdr:rowOff>152400</xdr:rowOff>
               </to>
@@ -22808,7 +22808,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="125953" r:id="rId8" name="cmdSpecifySets"/>
+        <control shapeId="125955" r:id="rId8" name="cmdCommUnit"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>
@@ -22881,18 +22881,18 @@
   <controls>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="80899" r:id="rId4" name="cmdProcUnits">
+        <control shapeId="80897" r:id="rId4" name="cmdSpecifySets">
           <controlPr defaultSize="0" autoLine="0" r:id="rId5">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>9525</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>19050</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>3</xdr:col>
-                <xdr:colOff>647700</xdr:colOff>
+                <xdr:col>4</xdr:col>
+                <xdr:colOff>1924050</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -22901,7 +22901,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="80899" r:id="rId4" name="cmdProcUnits"/>
+        <control shapeId="80897" r:id="rId4" name="cmdSpecifySets"/>
       </mc:Fallback>
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
@@ -22931,18 +22931,18 @@
     </mc:AlternateContent>
     <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
       <mc:Choice Requires="x14">
-        <control shapeId="80897" r:id="rId8" name="cmdSpecifySets">
+        <control shapeId="80899" r:id="rId8" name="cmdProcUnits">
           <controlPr defaultSize="0" autoLine="0" r:id="rId9">
             <anchor moveWithCells="1">
               <from>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>19050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>9525</xdr:colOff>
                 <xdr:row>3</xdr:row>
                 <xdr:rowOff>133350</xdr:rowOff>
               </from>
               <to>
-                <xdr:col>4</xdr:col>
-                <xdr:colOff>1924050</xdr:colOff>
+                <xdr:col>3</xdr:col>
+                <xdr:colOff>647700</xdr:colOff>
                 <xdr:row>5</xdr:row>
                 <xdr:rowOff>0</xdr:rowOff>
               </to>
@@ -22951,7 +22951,7 @@
         </control>
       </mc:Choice>
       <mc:Fallback>
-        <control shapeId="80897" r:id="rId8" name="cmdSpecifySets"/>
+        <control shapeId="80899" r:id="rId8" name="cmdProcUnits"/>
       </mc:Fallback>
     </mc:AlternateContent>
   </controls>

</xml_diff>

<commit_message>
SAIIA H2 model revisions.
Reset minimum investment constraints for diesel & petrol vehicles to zero by 2030.   

HCV6-9 diesel and ngas shaping of new capacity to avoid stranding of trucks from 2045 to meet NZ  objective. 

Future work: HCV1-5 trucks also stranding and requires a similar fix.
</commit_message>
<xml_diff>
--- a/SATIM/DataSpreadsheets/TCH_GRNEXP.xlsx
+++ b/SATIM/DataSpreadsheets/TCH_GRNEXP.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Models\SATIMGE\SATIM\DataSpreadsheets\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E5EAC687-D2BC-4ACC-ABFA-6AE3AE1797E9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{91FED8AF-BAAF-4557-AF17-0E7C7AA3AFD7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="796" activeTab="17" xr2:uid="{E4E4DEB2-CFB1-442C-9FC5-D51D154627BD}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" tabRatio="796" activeTab="14" xr2:uid="{E4E4DEB2-CFB1-442C-9FC5-D51D154627BD}"/>
   </bookViews>
   <sheets>
     <sheet name="ANSv2-692-Home" sheetId="9" r:id="rId1"/>
@@ -306,6 +306,31 @@
         </r>
       </text>
     </comment>
+    <comment ref="AS23" authorId="0" shapeId="0" xr:uid="{F606AC00-1855-47D5-9773-DC15AD04AD40}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Fadiel:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+Pt share of demand for autocatalysts removed.
+Note other PGMS such as Rh and Pd are not  factored. Needs a revisit.</t>
+        </r>
+      </text>
+    </comment>
     <comment ref="I25" authorId="0" shapeId="0" xr:uid="{E3D0E067-D854-4F66-B98D-7EB7F263DAC7}">
       <text>
         <r>
@@ -409,7 +434,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="578" uniqueCount="315">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="577" uniqueCount="315">
   <si>
     <t>Comment</t>
   </si>
@@ -1390,7 +1415,7 @@
     </r>
   </si>
   <si>
-    <t>Assuming that half of current use is for catalytic converters which are expected to disapear by 2050</t>
+    <t>Net platinum demand (tonnes) for the transtion</t>
   </si>
 </sst>
 </file>
@@ -1406,7 +1431,7 @@
     <numFmt numFmtId="168" formatCode="&quot;R&quot;#,##0.00000;[Red]\-&quot;R&quot;#,##0.00000"/>
     <numFmt numFmtId="169" formatCode="0.0"/>
   </numFmts>
-  <fonts count="53" x14ac:knownFonts="1">
+  <fonts count="55" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <name val="Arial"/>
@@ -1756,8 +1781,21 @@
       <name val="Arial"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="8"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="8"/>
+      <color theme="0" tint="-0.499984740745262"/>
+      <name val="Arial"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -1796,6 +1834,12 @@
     <fill>
       <patternFill patternType="solid">
         <fgColor theme="9" tint="0.79998168889431442"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="0" tint="-4.9989318521683403E-2"/>
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
@@ -2215,7 +2259,7 @@
     <xf numFmtId="9" fontId="6" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="239">
+  <cellXfs count="243">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="18" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -2572,15 +2616,19 @@
     <xf numFmtId="0" fontId="51" fillId="0" borderId="23" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
-    <xf numFmtId="1" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="20" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="165" fontId="20" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="10" fontId="0" fillId="0" borderId="0" xfId="18" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="24" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="53" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="54" fillId="8" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="53" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="54" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="1" fontId="21" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="21" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="21" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="165" fontId="21" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="169" fontId="21" fillId="7" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="51" fillId="0" borderId="22" xfId="12" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -11611,7 +11659,7 @@
   <dimension ref="A1:L11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B9" sqref="B9"/>
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="11.25" x14ac:dyDescent="0.2"/>
@@ -12637,10 +12685,10 @@
   <sheetPr codeName="Sheet31">
     <tabColor theme="4"/>
   </sheetPr>
-  <dimension ref="A1:AA15"/>
+  <dimension ref="A1:AA16"/>
   <sheetViews>
-    <sheetView topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="AA15" sqref="AA15"/>
+    <sheetView tabSelected="1" topLeftCell="F1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="L14" sqref="L14:T15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="9.140625" defaultRowHeight="11.25" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -12850,52 +12898,52 @@
       <c r="K7" s="12">
         <v>0</v>
       </c>
-      <c r="L7" s="12">
+      <c r="L7" s="217">
         <v>2012</v>
       </c>
-      <c r="M7" s="12">
+      <c r="M7" s="217">
         <v>2013</v>
       </c>
-      <c r="N7" s="12">
+      <c r="N7" s="217">
         <v>2014</v>
       </c>
-      <c r="O7" s="12">
+      <c r="O7" s="217">
         <v>2015</v>
       </c>
-      <c r="P7" s="12">
+      <c r="P7" s="217">
         <v>2016</v>
       </c>
-      <c r="Q7" s="12">
+      <c r="Q7" s="217">
         <v>2017</v>
       </c>
-      <c r="R7" s="12">
+      <c r="R7" s="217">
         <v>2018</v>
       </c>
-      <c r="S7" s="12">
+      <c r="S7" s="217">
         <v>2019</v>
       </c>
-      <c r="T7" s="214">
+      <c r="T7" s="218">
         <v>2020</v>
       </c>
-      <c r="U7" s="214">
+      <c r="U7" s="221">
         <v>2025</v>
       </c>
-      <c r="V7" s="214">
+      <c r="V7" s="221">
         <v>2030</v>
       </c>
-      <c r="W7" s="214">
+      <c r="W7" s="221">
         <v>2035</v>
       </c>
-      <c r="X7" s="214">
+      <c r="X7" s="221">
         <v>2039</v>
       </c>
-      <c r="Y7" s="214">
+      <c r="Y7" s="221">
         <v>2040</v>
       </c>
-      <c r="Z7" s="214">
+      <c r="Z7" s="221">
         <v>2045</v>
       </c>
-      <c r="AA7" s="214">
+      <c r="AA7" s="221">
         <v>2050</v>
       </c>
     </row>
@@ -12909,14 +12957,22 @@
       <c r="F8" s="110"/>
       <c r="G8" s="198"/>
       <c r="H8" s="106"/>
-      <c r="T8" s="214"/>
-      <c r="U8" s="214"/>
-      <c r="V8" s="214"/>
-      <c r="W8" s="214"/>
-      <c r="X8" s="214"/>
-      <c r="Y8" s="214"/>
-      <c r="Z8" s="214"/>
-      <c r="AA8" s="214"/>
+      <c r="L8" s="217"/>
+      <c r="M8" s="217"/>
+      <c r="N8" s="217"/>
+      <c r="O8" s="217"/>
+      <c r="P8" s="217"/>
+      <c r="Q8" s="217"/>
+      <c r="R8" s="217"/>
+      <c r="S8" s="217"/>
+      <c r="T8" s="218"/>
+      <c r="U8" s="221"/>
+      <c r="V8" s="221"/>
+      <c r="W8" s="221"/>
+      <c r="X8" s="221"/>
+      <c r="Y8" s="221"/>
+      <c r="Z8" s="221"/>
+      <c r="AA8" s="221"/>
     </row>
     <row r="9" spans="1:27" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B9" s="12" t="str">
@@ -12952,57 +13008,57 @@
       <c r="K9" s="164">
         <v>5</v>
       </c>
-      <c r="L9" s="164">
+      <c r="L9" s="219">
         <f>'Exports summary'!G7</f>
         <v>124.69952392131813</v>
       </c>
-      <c r="M9" s="164">
+      <c r="M9" s="219">
         <f>'Exports summary'!H7</f>
         <v>130.71131620168498</v>
       </c>
-      <c r="N9" s="164">
+      <c r="N9" s="219">
         <f>'Exports summary'!I7</f>
         <v>84.02169487089688</v>
       </c>
-      <c r="O9" s="164">
+      <c r="O9" s="219">
         <f>'Exports summary'!J7</f>
         <v>133.92546693812523</v>
       </c>
-      <c r="P9" s="164">
+      <c r="P9" s="219">
         <f>'Exports summary'!K7</f>
         <v>127.71131620168498</v>
       </c>
-      <c r="Q9" s="164">
+      <c r="Q9" s="219">
         <f>'Exports summary'!L7</f>
         <v>125.30659928953824</v>
       </c>
-      <c r="R9" s="164">
+      <c r="R9" s="219">
         <v>132.92896377787815</v>
       </c>
-      <c r="S9" s="164">
+      <c r="S9" s="219">
         <v>143.56859209868344</v>
       </c>
-      <c r="T9" s="215">
+      <c r="T9" s="220">
         <v>107.43885384834891</v>
       </c>
-      <c r="U9" s="216">
+      <c r="U9" s="222">
         <f>MEDIAN(R9:S9)</f>
         <v>138.2487779382808</v>
       </c>
-      <c r="V9" s="216">
+      <c r="V9" s="226">
         <f>Scenarios!AQ25</f>
         <v>140.62042040052222</v>
       </c>
-      <c r="W9" s="217"/>
-      <c r="X9" s="217"/>
-      <c r="Y9" s="216">
+      <c r="W9" s="223"/>
+      <c r="X9" s="223"/>
+      <c r="Y9" s="222">
         <f>Scenarios!AR25</f>
-        <v>135.93802235772677</v>
-      </c>
-      <c r="Z9" s="216"/>
-      <c r="AA9" s="216">
+        <v>170.13629509932673</v>
+      </c>
+      <c r="Z9" s="222"/>
+      <c r="AA9" s="222">
         <f>Scenarios!AS25</f>
-        <v>504.64573096167442</v>
+        <v>526.83014240445232</v>
       </c>
     </row>
     <row r="10" spans="1:27" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
@@ -13039,49 +13095,49 @@
       <c r="K10" s="164">
         <v>5</v>
       </c>
-      <c r="L10" s="164">
+      <c r="L10" s="219">
         <f>'Exports summary'!G8</f>
         <v>101.30047607868187</v>
       </c>
-      <c r="M10" s="164">
+      <c r="M10" s="219">
         <f>'Exports summary'!H8</f>
         <v>105.28868379831502</v>
       </c>
-      <c r="N10" s="164">
+      <c r="N10" s="219">
         <f>'Exports summary'!I8</f>
         <v>74.97830512910312</v>
       </c>
-      <c r="O10" s="164">
+      <c r="O10" s="219">
         <f>'Exports summary'!J8</f>
         <v>110.07453306187479</v>
       </c>
-      <c r="P10" s="164">
+      <c r="P10" s="219">
         <f>'Exports summary'!K8</f>
         <v>105.28868379831502</v>
       </c>
-      <c r="Q10" s="164">
+      <c r="Q10" s="219">
         <f>'Exports summary'!L8</f>
         <v>103.69340071046176</v>
       </c>
-      <c r="R10" s="164"/>
-      <c r="S10" s="164"/>
-      <c r="T10" s="215">
+      <c r="R10" s="219"/>
+      <c r="S10" s="219"/>
+      <c r="T10" s="220">
         <f>Q10</f>
         <v>103.69340071046176</v>
       </c>
-      <c r="U10" s="216">
+      <c r="U10" s="222">
         <f>'Exports summary'!O8</f>
         <v>103.69340071046176</v>
       </c>
-      <c r="V10" s="216">
+      <c r="V10" s="222">
         <f>'Exports summary'!P8</f>
         <v>103.69340071046176</v>
       </c>
-      <c r="W10" s="216"/>
-      <c r="X10" s="216"/>
-      <c r="Y10" s="216"/>
-      <c r="Z10" s="216"/>
-      <c r="AA10" s="216">
+      <c r="W10" s="222"/>
+      <c r="X10" s="222"/>
+      <c r="Y10" s="222"/>
+      <c r="Z10" s="222"/>
+      <c r="AA10" s="222">
         <f>'Exports summary'!T8</f>
         <v>103.69340071046176</v>
       </c>
@@ -13120,32 +13176,39 @@
       <c r="K11" s="12">
         <v>5</v>
       </c>
-      <c r="L11" s="12">
+      <c r="L11" s="217">
         <v>2.7578</v>
       </c>
-      <c r="T11" s="214"/>
-      <c r="U11" s="218"/>
-      <c r="V11" s="218">
+      <c r="M11" s="217"/>
+      <c r="N11" s="217"/>
+      <c r="O11" s="217"/>
+      <c r="P11" s="217"/>
+      <c r="Q11" s="217"/>
+      <c r="R11" s="217"/>
+      <c r="S11" s="217"/>
+      <c r="T11" s="218"/>
+      <c r="U11" s="224"/>
+      <c r="V11" s="224">
         <f>'Exports summary'!P16</f>
         <v>2.7578253706754534</v>
       </c>
-      <c r="W11" s="217" t="str">
+      <c r="W11" s="223" t="str">
         <f>'Exports summary'!Q16</f>
         <v/>
       </c>
-      <c r="X11" s="217" t="str">
+      <c r="X11" s="223" t="str">
         <f>'Exports summary'!R16</f>
         <v/>
       </c>
-      <c r="Y11" s="217" t="str">
+      <c r="Y11" s="223" t="str">
         <f>'Exports summary'!R16</f>
         <v/>
       </c>
-      <c r="Z11" s="217" t="str">
+      <c r="Z11" s="223" t="str">
         <f>'Exports summary'!S16</f>
         <v/>
       </c>
-      <c r="AA11" s="217">
+      <c r="AA11" s="223">
         <f>'Exports summary'!T16</f>
         <v>124.155</v>
       </c>
@@ -13184,32 +13247,40 @@
       <c r="K12" s="12">
         <v>5</v>
       </c>
-      <c r="T12" s="214"/>
-      <c r="U12" s="217" t="str">
+      <c r="L12" s="217"/>
+      <c r="M12" s="217"/>
+      <c r="N12" s="217"/>
+      <c r="O12" s="217"/>
+      <c r="P12" s="217"/>
+      <c r="Q12" s="217"/>
+      <c r="R12" s="217"/>
+      <c r="S12" s="217"/>
+      <c r="T12" s="218"/>
+      <c r="U12" s="223" t="str">
         <f>'Exports summary'!O11</f>
         <v/>
       </c>
-      <c r="V12" s="217">
+      <c r="V12" s="223">
         <f>'Exports summary'!P11</f>
         <v>1</v>
       </c>
-      <c r="W12" s="217" t="str">
+      <c r="W12" s="223" t="str">
         <f>'Exports summary'!Q11</f>
         <v/>
       </c>
-      <c r="X12" s="217" t="str">
+      <c r="X12" s="223" t="str">
         <f>'Exports summary'!R11</f>
         <v/>
       </c>
-      <c r="Y12" s="217" t="str">
+      <c r="Y12" s="223" t="str">
         <f>'Exports summary'!R11</f>
         <v/>
       </c>
-      <c r="Z12" s="217" t="str">
+      <c r="Z12" s="223" t="str">
         <f>'Exports summary'!S11</f>
         <v/>
       </c>
-      <c r="AA12" s="217">
+      <c r="AA12" s="223">
         <f>'Exports summary'!T11</f>
         <v>14</v>
       </c>
@@ -13248,22 +13319,30 @@
       <c r="K13" s="12">
         <v>5</v>
       </c>
-      <c r="T13" s="214"/>
-      <c r="U13" s="216"/>
-      <c r="V13" s="216"/>
-      <c r="W13" s="216"/>
-      <c r="X13" s="216">
+      <c r="L13" s="217"/>
+      <c r="M13" s="217"/>
+      <c r="N13" s="217"/>
+      <c r="O13" s="217"/>
+      <c r="P13" s="217"/>
+      <c r="Q13" s="217"/>
+      <c r="R13" s="217"/>
+      <c r="S13" s="217"/>
+      <c r="T13" s="218"/>
+      <c r="U13" s="222"/>
+      <c r="V13" s="222"/>
+      <c r="W13" s="222"/>
+      <c r="X13" s="222">
         <v>0</v>
       </c>
-      <c r="Y13" s="216">
+      <c r="Y13" s="222">
         <f>Scenarios!AF16</f>
         <v>5.0430461919999994</v>
       </c>
-      <c r="Z13" s="216">
+      <c r="Z13" s="222">
         <f>Y13</f>
         <v>5.0430461919999994</v>
       </c>
-      <c r="AA13" s="216">
+      <c r="AA13" s="222">
         <f>Scenarios!AG16</f>
         <v>10.086092383999999</v>
       </c>
@@ -13302,20 +13381,34 @@
       <c r="K14" s="12">
         <v>5</v>
       </c>
-      <c r="T14" s="214"/>
-      <c r="U14" s="217"/>
-      <c r="V14" s="217">
+      <c r="L14" s="217">
+        <v>0</v>
+      </c>
+      <c r="M14" s="217"/>
+      <c r="N14" s="217"/>
+      <c r="O14" s="217"/>
+      <c r="P14" s="217"/>
+      <c r="Q14" s="217">
+        <v>0</v>
+      </c>
+      <c r="R14" s="217"/>
+      <c r="S14" s="217"/>
+      <c r="T14" s="218">
+        <v>0</v>
+      </c>
+      <c r="U14" s="223"/>
+      <c r="V14" s="223">
         <f>Scenarios!R6</f>
         <v>0.2</v>
       </c>
-      <c r="W14" s="214"/>
-      <c r="X14" s="214"/>
-      <c r="Y14" s="219">
+      <c r="W14" s="221"/>
+      <c r="X14" s="221"/>
+      <c r="Y14" s="225">
         <f>Scenarios!S6</f>
         <v>2.3572743999999997</v>
       </c>
-      <c r="Z14" s="219"/>
-      <c r="AA14" s="219">
+      <c r="Z14" s="225"/>
+      <c r="AA14" s="225">
         <f>Scenarios!T6</f>
         <v>21.333332000000002</v>
       </c>
@@ -13354,23 +13447,57 @@
       <c r="K15" s="12">
         <v>5</v>
       </c>
-      <c r="T15" s="214"/>
-      <c r="U15" s="217">
+      <c r="L15" s="217">
         <v>0</v>
       </c>
-      <c r="V15" s="218">
+      <c r="M15" s="217"/>
+      <c r="N15" s="217"/>
+      <c r="O15" s="217"/>
+      <c r="P15" s="217"/>
+      <c r="Q15" s="217">
+        <v>0</v>
+      </c>
+      <c r="R15" s="217"/>
+      <c r="S15" s="217"/>
+      <c r="T15" s="218">
+        <v>0</v>
+      </c>
+      <c r="U15" s="223">
+        <v>0</v>
+      </c>
+      <c r="V15" s="224">
         <f>Scenarios!U6</f>
         <v>2.5600000000000001E-2</v>
       </c>
-      <c r="Y15" s="218">
+      <c r="W15" s="221"/>
+      <c r="X15" s="221"/>
+      <c r="Y15" s="224">
         <f>Scenarios!V6</f>
         <v>7.7933579200000009</v>
       </c>
-      <c r="Z15" s="217"/>
-      <c r="AA15" s="218">
+      <c r="Z15" s="223"/>
+      <c r="AA15" s="224">
         <f>Scenarios!W6</f>
         <v>309.96310400000004</v>
       </c>
+    </row>
+    <row r="16" spans="1:27" ht="11.25" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="L16" s="217"/>
+      <c r="M16" s="217"/>
+      <c r="N16" s="217"/>
+      <c r="O16" s="217"/>
+      <c r="P16" s="217"/>
+      <c r="Q16" s="217"/>
+      <c r="R16" s="217"/>
+      <c r="S16" s="217"/>
+      <c r="T16" s="217"/>
+      <c r="U16" s="221"/>
+      <c r="V16" s="221"/>
+      <c r="W16" s="221"/>
+      <c r="X16" s="221"/>
+      <c r="Y16" s="221"/>
+      <c r="Z16" s="221"/>
+      <c r="AA16" s="221"/>
     </row>
   </sheetData>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
@@ -14013,7 +14140,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="D16" sqref="D16"/>
+      <selection pane="bottomLeft" activeCell="L8" sqref="L8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.85546875" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -14454,8 +14581,8 @@
   </sheetPr>
   <dimension ref="B2:AW53"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
-      <selection activeCell="W6" sqref="W6"/>
+    <sheetView topLeftCell="AE1" workbookViewId="0">
+      <selection activeCell="AR29" sqref="AR29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -14479,8 +14606,8 @@
       <c r="AA2" s="89" t="s">
         <v>267</v>
       </c>
-      <c r="AL2" t="s">
-        <v>295</v>
+      <c r="AL2" s="89" t="s">
+        <v>314</v>
       </c>
     </row>
     <row r="3" spans="2:42" ht="57.75" thickBot="1" x14ac:dyDescent="0.25">
@@ -14490,19 +14617,19 @@
       <c r="C3" s="1" t="s">
         <v>15</v>
       </c>
-      <c r="Q3" s="237" t="s">
+      <c r="Q3" s="241" t="s">
         <v>260</v>
       </c>
       <c r="R3" s="199"/>
-      <c r="S3" s="223" t="s">
+      <c r="S3" s="227" t="s">
         <v>261</v>
       </c>
-      <c r="T3" s="224"/>
+      <c r="T3" s="228"/>
       <c r="U3" s="199"/>
-      <c r="V3" s="223" t="s">
+      <c r="V3" s="227" t="s">
         <v>262</v>
       </c>
-      <c r="W3" s="224"/>
+      <c r="W3" s="228"/>
       <c r="AC3" s="211"/>
       <c r="AL3" s="211" t="s">
         <v>295</v>
@@ -14524,7 +14651,7 @@
       <c r="C4" s="176" t="s">
         <v>211</v>
       </c>
-      <c r="Q4" s="238"/>
+      <c r="Q4" s="242"/>
       <c r="R4" s="200">
         <v>2030</v>
       </c>
@@ -14658,39 +14785,39 @@
       <c r="W7" s="205">
         <v>818.30256000000008</v>
       </c>
-      <c r="AL7" s="228" t="s">
+      <c r="AL7" s="232" t="s">
         <v>298</v>
       </c>
-      <c r="AM7" s="229"/>
-      <c r="AN7" s="229"/>
-      <c r="AO7" s="230"/>
+      <c r="AM7" s="233"/>
+      <c r="AN7" s="233"/>
+      <c r="AO7" s="234"/>
     </row>
     <row r="8" spans="2:42" ht="13.5" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B8" s="175"/>
       <c r="C8" s="175"/>
-      <c r="Q8" s="225" t="s">
+      <c r="Q8" s="229" t="s">
         <v>299</v>
       </c>
-      <c r="R8" s="226"/>
-      <c r="S8" s="226"/>
-      <c r="T8" s="226"/>
-      <c r="U8" s="226"/>
-      <c r="V8" s="226"/>
-      <c r="W8" s="227"/>
-      <c r="AL8" s="231" t="s">
+      <c r="R8" s="230"/>
+      <c r="S8" s="230"/>
+      <c r="T8" s="230"/>
+      <c r="U8" s="230"/>
+      <c r="V8" s="230"/>
+      <c r="W8" s="231"/>
+      <c r="AL8" s="235" t="s">
         <v>296</v>
       </c>
-      <c r="AM8" s="232"/>
-      <c r="AN8" s="232"/>
-      <c r="AO8" s="233"/>
+      <c r="AM8" s="236"/>
+      <c r="AN8" s="236"/>
+      <c r="AO8" s="237"/>
     </row>
     <row r="9" spans="2:42" ht="21.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="AL9" s="234" t="s">
+      <c r="AL9" s="238" t="s">
         <v>297</v>
       </c>
-      <c r="AM9" s="235"/>
-      <c r="AN9" s="235"/>
-      <c r="AO9" s="236"/>
+      <c r="AM9" s="239"/>
+      <c r="AN9" s="239"/>
+      <c r="AO9" s="240"/>
     </row>
     <row r="14" spans="2:42" x14ac:dyDescent="0.2">
       <c r="AA14" s="100" t="s">
@@ -14799,7 +14926,7 @@
       <c r="AB16" t="s">
         <v>116</v>
       </c>
-      <c r="AC16" s="221" t="s">
+      <c r="AC16" s="215" t="s">
         <v>271</v>
       </c>
       <c r="AF16" s="182">
@@ -15140,20 +15267,17 @@
         <v>99.500022283199996</v>
       </c>
       <c r="AQ24" s="148">
-        <f t="shared" ref="AQ24:AS26" si="4">MEDIAN($AN24:$AP24)+AM4</f>
         <v>140.45051883561732</v>
       </c>
       <c r="AR24" s="148">
-        <f t="shared" si="4"/>
         <v>137.99364982983465</v>
       </c>
       <c r="AS24" s="148">
-        <f t="shared" si="4"/>
-        <v>137.93364982983465</v>
+        <v>91.72151578941255</v>
       </c>
       <c r="AU24">
         <f>AS24/AM24</f>
-        <v>1.0083378396918803</v>
+        <v>0.67051278059022568</v>
       </c>
     </row>
     <row r="25" spans="2:49" ht="15" x14ac:dyDescent="0.25">
@@ -15207,7 +15331,7 @@
         <v>Medium</v>
       </c>
       <c r="AM25">
-        <f t="shared" ref="AM25:AM26" si="5">MEDIAN(AN25:AP25)</f>
+        <f t="shared" ref="AM25:AM26" si="4">MEDIAN(AN25:AP25)</f>
         <v>136.7930909664</v>
       </c>
       <c r="AN25">
@@ -15215,7 +15339,7 @@
         <v>138.9392308656</v>
       </c>
       <c r="AO25">
-        <f t="shared" ref="AO25:AP26" si="6">AO24</f>
+        <f t="shared" ref="AO25:AP26" si="5">AO24</f>
         <v>136.7930909664</v>
       </c>
       <c r="AP25">
@@ -15223,24 +15347,19 @@
         <v>99.500022283199996</v>
       </c>
       <c r="AQ25" s="148">
-        <f t="shared" si="4"/>
         <v>140.62042040052222</v>
       </c>
       <c r="AR25" s="148">
-        <f>MEDIAN($AN25:$AP25)*0.75+AN5</f>
-        <v>135.93802235772677</v>
+        <v>170.13629509932673</v>
       </c>
       <c r="AS25" s="148">
-        <f>MEDIAN($AN25:$AP25)*0.5+AO5</f>
-        <v>504.64573096167442</v>
+        <v>526.83014240445232</v>
       </c>
       <c r="AU25">
         <f>AS25/AM25</f>
-        <v>3.6891170993835409</v>
-      </c>
-      <c r="AW25" s="89" t="s">
-        <v>314</v>
-      </c>
+        <v>3.8512920402818862</v>
+      </c>
+      <c r="AW25" s="89"/>
     </row>
     <row r="26" spans="2:49" x14ac:dyDescent="0.2">
       <c r="I26">
@@ -15273,7 +15392,7 @@
         <v>High</v>
       </c>
       <c r="AM26">
-        <f t="shared" si="5"/>
+        <f t="shared" si="4"/>
         <v>136.7930909664</v>
       </c>
       <c r="AN26">
@@ -15281,28 +15400,25 @@
         <v>138.9392308656</v>
       </c>
       <c r="AO26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>136.7930909664</v>
       </c>
       <c r="AP26">
-        <f t="shared" si="6"/>
+        <f t="shared" si="5"/>
         <v>99.500022283199996</v>
       </c>
       <c r="AQ26" s="148">
-        <f t="shared" si="4"/>
         <v>196.35923549853283</v>
       </c>
       <c r="AR26" s="148">
-        <f t="shared" si="4"/>
         <v>679.22700966264995</v>
       </c>
       <c r="AS26" s="148">
-        <f t="shared" si="4"/>
-        <v>1509.82947857265</v>
+        <v>1463.6173445322279</v>
       </c>
       <c r="AU26">
         <f>AS26/AM26</f>
-        <v>11.037322630157572</v>
+        <v>10.699497571055916</v>
       </c>
     </row>
     <row r="27" spans="2:49" x14ac:dyDescent="0.2">
@@ -15738,12 +15854,12 @@
       <c r="AA42" s="89" t="s">
         <v>306</v>
       </c>
-      <c r="AE42" s="220">
-        <f t="shared" ref="AE42" si="7">AE32/SUM(AE25:AE39)</f>
+      <c r="AE42" s="214">
+        <f t="shared" ref="AE42" si="6">AE32/SUM(AE25:AE39)</f>
         <v>4.6157376605006142E-2</v>
       </c>
-      <c r="AF42" s="220"/>
-      <c r="AG42" s="220">
+      <c r="AF42" s="214"/>
+      <c r="AG42" s="214">
         <f>AG32/SUM(AG25:AG39)</f>
         <v>4.5196011737906945E-2</v>
       </c>
@@ -15830,7 +15946,7 @@
       </c>
     </row>
     <row r="53" spans="17:22" ht="15" x14ac:dyDescent="0.25">
-      <c r="Q53" s="222" t="s">
+      <c r="Q53" s="216" t="s">
         <v>313</v>
       </c>
     </row>

</xml_diff>